<commit_message>
updated docs and waveLogo
</commit_message>
<xml_diff>
--- a/examples/logo.xlsx
+++ b/examples/logo.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raskin1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\raskin1\codes\yggdrasil\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4886E397-4746-4123-BDAD-2411574D04A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0018E6DE-1F03-4E81-9CC2-B32DCF6AEBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="1020" windowWidth="31290" windowHeight="16725" xr2:uid="{6C904F15-F3DC-4125-804F-43E284D343AD}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="38700" windowHeight="15345" activeTab="1" xr2:uid="{6C904F15-F3DC-4125-804F-43E284D343AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,8 +46,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -56,6 +65,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -72,9 +105,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77A645E-27DC-4567-A593-D511F1EC241A}">
   <dimension ref="A1:BD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BD3" sqref="BD3:BD34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +600,7 @@
         <v>20</v>
       </c>
       <c r="BA3">
-        <f t="shared" ref="AZ3:BB3" si="0">4*AV3</f>
+        <f t="shared" ref="BA3" si="0">4*AV3</f>
         <v>20</v>
       </c>
       <c r="BB3">
@@ -1815,4 +1855,2615 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD76C112-254A-4FDB-9AA5-428B7BE0CB6D}">
+  <dimension ref="A1:CC42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="CC30" sqref="CC30:CC35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="77" max="77" width="5.5703125" customWidth="1"/>
+    <col min="81" max="81" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+      <c r="R1">
+        <v>18</v>
+      </c>
+      <c r="S1">
+        <v>19</v>
+      </c>
+      <c r="T1">
+        <v>20</v>
+      </c>
+      <c r="U1">
+        <v>21</v>
+      </c>
+      <c r="V1">
+        <v>22</v>
+      </c>
+      <c r="W1">
+        <v>23</v>
+      </c>
+      <c r="X1">
+        <v>24</v>
+      </c>
+      <c r="Y1">
+        <v>25</v>
+      </c>
+      <c r="Z1">
+        <v>26</v>
+      </c>
+      <c r="AA1">
+        <v>27</v>
+      </c>
+      <c r="AB1">
+        <v>28</v>
+      </c>
+      <c r="AC1">
+        <v>29</v>
+      </c>
+      <c r="AD1">
+        <v>30</v>
+      </c>
+      <c r="AE1">
+        <v>31</v>
+      </c>
+      <c r="AF1">
+        <v>32</v>
+      </c>
+      <c r="AG1">
+        <v>33</v>
+      </c>
+      <c r="AH1">
+        <v>34</v>
+      </c>
+      <c r="AI1">
+        <v>35</v>
+      </c>
+      <c r="AJ1">
+        <v>36</v>
+      </c>
+      <c r="AK1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="AU3">
+        <v>3</v>
+      </c>
+      <c r="AV3">
+        <v>8</v>
+      </c>
+      <c r="AW3">
+        <v>4</v>
+      </c>
+      <c r="AX3">
+        <v>12</v>
+      </c>
+      <c r="AZ3">
+        <f>4*AU3</f>
+        <v>12</v>
+      </c>
+      <c r="BA3">
+        <f>4*(20-AX3)</f>
+        <v>32</v>
+      </c>
+      <c r="BB3">
+        <f t="shared" ref="BB3:BB35" si="0">4*AW3</f>
+        <v>16</v>
+      </c>
+      <c r="BC3">
+        <f>4*(20-AV3)</f>
+        <v>48</v>
+      </c>
+      <c r="BE3" s="7" t="str">
+        <f>"box.addBox(Vector2d("&amp;AZ3&amp;","&amp;BA3&amp;"),Vector2d("&amp;BB3&amp;","&amp;BC3&amp;"))"</f>
+        <v>box.addBox(Vector2d(12,32),Vector2d(16,48))</v>
+      </c>
+      <c r="BF3" s="6"/>
+      <c r="BV3">
+        <v>5</v>
+      </c>
+      <c r="BW3">
+        <v>4</v>
+      </c>
+      <c r="BY3">
+        <f>BV3*4</f>
+        <v>20</v>
+      </c>
+      <c r="BZ3">
+        <f>4*(20-BW3)</f>
+        <v>64</v>
+      </c>
+      <c r="CC3" t="str">
+        <f>"locations.append(["&amp;BY3&amp;","&amp;BZ3&amp;"])"</f>
+        <v>locations.append([20,64])</v>
+      </c>
+    </row>
+    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="E4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AU4">
+        <v>3</v>
+      </c>
+      <c r="AV4">
+        <v>13</v>
+      </c>
+      <c r="AW4">
+        <v>4</v>
+      </c>
+      <c r="AX4">
+        <v>15</v>
+      </c>
+      <c r="AZ4">
+        <f t="shared" ref="AZ4:AZ35" si="1">4*AU4</f>
+        <v>12</v>
+      </c>
+      <c r="BA4">
+        <f t="shared" ref="BA4:BA35" si="2">4*(20-AX4)</f>
+        <v>20</v>
+      </c>
+      <c r="BB4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="BC4">
+        <f t="shared" ref="BC4:BC35" si="3">4*(20-AV4)</f>
+        <v>28</v>
+      </c>
+      <c r="BE4" s="7" t="str">
+        <f t="shared" ref="BE4:BE35" si="4">"box.addBox(Vector2d("&amp;AZ4&amp;","&amp;BA4&amp;"),Vector2d("&amp;BB4&amp;","&amp;BC4&amp;"))"</f>
+        <v>box.addBox(Vector2d(12,20),Vector2d(16,28))</v>
+      </c>
+      <c r="BF4" s="6"/>
+      <c r="BV4">
+        <v>9</v>
+      </c>
+      <c r="BW4">
+        <v>4</v>
+      </c>
+      <c r="BY4">
+        <f t="shared" ref="BY4:BY28" si="5">BV4*4</f>
+        <v>36</v>
+      </c>
+      <c r="BZ4">
+        <f t="shared" ref="BZ4:BZ28" si="6">4*(20-BW4)</f>
+        <v>64</v>
+      </c>
+      <c r="CC4" t="str">
+        <f t="shared" ref="CC4:CC28" si="7">"locations.append(["&amp;BY4&amp;","&amp;BZ4&amp;"])"</f>
+        <v>locations.append([36,64])</v>
+      </c>
+    </row>
+    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="2"/>
+      <c r="AU5">
+        <v>4</v>
+      </c>
+      <c r="AV5">
+        <v>7</v>
+      </c>
+      <c r="AW5">
+        <v>5</v>
+      </c>
+      <c r="AX5">
+        <v>8</v>
+      </c>
+      <c r="AZ5">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="BA5">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="BB5">
+        <f t="shared" ref="BB5:BB42" si="8">4*AW5</f>
+        <v>20</v>
+      </c>
+      <c r="BC5">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="BE5" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>box.addBox(Vector2d(16,48),Vector2d(20,52))</v>
+      </c>
+      <c r="BF5" s="6"/>
+      <c r="BV5">
+        <v>13</v>
+      </c>
+      <c r="BW5">
+        <v>4</v>
+      </c>
+      <c r="BY5">
+        <f t="shared" si="5"/>
+        <v>52</v>
+      </c>
+      <c r="BZ5">
+        <f t="shared" si="6"/>
+        <v>64</v>
+      </c>
+      <c r="CC5" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([52,64])</v>
+      </c>
+    </row>
+    <row r="6" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="4"/>
+      <c r="AU6">
+        <v>6</v>
+      </c>
+      <c r="AV6">
+        <v>7</v>
+      </c>
+      <c r="AW6">
+        <v>7</v>
+      </c>
+      <c r="AX6">
+        <v>8</v>
+      </c>
+      <c r="AZ6">
+        <f t="shared" ref="AZ6:AZ42" si="9">4*AU6</f>
+        <v>24</v>
+      </c>
+      <c r="BA6">
+        <f t="shared" ref="BA6:BA42" si="10">4*(20-AX6)</f>
+        <v>48</v>
+      </c>
+      <c r="BB6">
+        <f t="shared" si="8"/>
+        <v>28</v>
+      </c>
+      <c r="BC6">
+        <f t="shared" ref="BC6:BC42" si="11">4*(20-AV6)</f>
+        <v>52</v>
+      </c>
+      <c r="BE6" s="7" t="str">
+        <f t="shared" ref="BE6:BE42" si="12">"box.addBox(Vector2d("&amp;AZ6&amp;","&amp;BA6&amp;"),Vector2d("&amp;BB6&amp;","&amp;BC6&amp;"))"</f>
+        <v>box.addBox(Vector2d(24,48),Vector2d(28,52))</v>
+      </c>
+      <c r="BF6" s="6"/>
+      <c r="BV6">
+        <v>21</v>
+      </c>
+      <c r="BW6">
+        <v>4</v>
+      </c>
+      <c r="BY6">
+        <f t="shared" si="5"/>
+        <v>84</v>
+      </c>
+      <c r="BZ6">
+        <f t="shared" si="6"/>
+        <v>64</v>
+      </c>
+      <c r="CC6" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([84,64])</v>
+      </c>
+    </row>
+    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="4"/>
+      <c r="AU7">
+        <v>4</v>
+      </c>
+      <c r="AV7">
+        <v>12</v>
+      </c>
+      <c r="AW7">
+        <v>5</v>
+      </c>
+      <c r="AX7">
+        <v>13</v>
+      </c>
+      <c r="AZ7">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="BA7">
+        <f t="shared" si="10"/>
+        <v>28</v>
+      </c>
+      <c r="BB7">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="BC7">
+        <f t="shared" si="11"/>
+        <v>32</v>
+      </c>
+      <c r="BE7" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(16,28),Vector2d(20,32))</v>
+      </c>
+      <c r="BF7" s="6"/>
+      <c r="BV7">
+        <v>25</v>
+      </c>
+      <c r="BW7">
+        <v>4</v>
+      </c>
+      <c r="BY7">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="BZ7">
+        <f t="shared" si="6"/>
+        <v>64</v>
+      </c>
+      <c r="CC7" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([100,64])</v>
+      </c>
+    </row>
+    <row r="8" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="4"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="4"/>
+      <c r="AU8">
+        <v>5</v>
+      </c>
+      <c r="AV8">
+        <v>8</v>
+      </c>
+      <c r="AW8">
+        <v>6</v>
+      </c>
+      <c r="AX8">
+        <v>10</v>
+      </c>
+      <c r="AZ8">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
+      <c r="BA8">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="BB8">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+      <c r="BC8">
+        <f t="shared" si="11"/>
+        <v>48</v>
+      </c>
+      <c r="BE8" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(20,40),Vector2d(24,48))</v>
+      </c>
+      <c r="BF8" s="6"/>
+      <c r="BV8">
+        <v>29</v>
+      </c>
+      <c r="BW8">
+        <v>4</v>
+      </c>
+      <c r="BY8">
+        <f t="shared" si="5"/>
+        <v>116</v>
+      </c>
+      <c r="BZ8">
+        <f t="shared" si="6"/>
+        <v>64</v>
+      </c>
+      <c r="CC8" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([116,64])</v>
+      </c>
+    </row>
+    <row r="9" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="5"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="4"/>
+      <c r="AU9">
+        <v>4</v>
+      </c>
+      <c r="AV9">
+        <v>15</v>
+      </c>
+      <c r="AW9">
+        <v>7</v>
+      </c>
+      <c r="AX9">
+        <v>16</v>
+      </c>
+      <c r="AZ9">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="BA9">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="BB9">
+        <f t="shared" si="8"/>
+        <v>28</v>
+      </c>
+      <c r="BC9">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="BE9" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(16,16),Vector2d(28,20))</v>
+      </c>
+      <c r="BF9" s="6"/>
+      <c r="BV9">
+        <v>33</v>
+      </c>
+      <c r="BW9">
+        <v>4</v>
+      </c>
+      <c r="BY9">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+      <c r="BZ9">
+        <f t="shared" si="6"/>
+        <v>64</v>
+      </c>
+      <c r="CC9" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([132,64])</v>
+      </c>
+    </row>
+    <row r="10" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="4"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="4"/>
+      <c r="AU10">
+        <v>7</v>
+      </c>
+      <c r="AV10">
+        <v>8</v>
+      </c>
+      <c r="AW10">
+        <v>8</v>
+      </c>
+      <c r="AX10">
+        <v>15</v>
+      </c>
+      <c r="AZ10">
+        <f t="shared" si="9"/>
+        <v>28</v>
+      </c>
+      <c r="BA10">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="BB10">
+        <f t="shared" si="8"/>
+        <v>32</v>
+      </c>
+      <c r="BC10">
+        <f t="shared" si="11"/>
+        <v>48</v>
+      </c>
+      <c r="BE10" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(28,20),Vector2d(32,48))</v>
+      </c>
+      <c r="BF10" s="6"/>
+      <c r="BV10">
+        <v>32</v>
+      </c>
+      <c r="BW10">
+        <v>7</v>
+      </c>
+      <c r="BY10">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+      <c r="BZ10">
+        <f t="shared" si="6"/>
+        <v>52</v>
+      </c>
+      <c r="CC10" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([128,52])</v>
+      </c>
+    </row>
+    <row r="11" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="4"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="4"/>
+      <c r="AU11">
+        <v>11</v>
+      </c>
+      <c r="AV11">
+        <v>8</v>
+      </c>
+      <c r="AW11">
+        <v>12</v>
+      </c>
+      <c r="AX11">
+        <v>15</v>
+      </c>
+      <c r="AZ11">
+        <f t="shared" si="9"/>
+        <v>44</v>
+      </c>
+      <c r="BA11">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="BB11">
+        <f t="shared" si="8"/>
+        <v>48</v>
+      </c>
+      <c r="BC11">
+        <f t="shared" si="11"/>
+        <v>48</v>
+      </c>
+      <c r="BE11" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(44,20),Vector2d(48,48))</v>
+      </c>
+      <c r="BF11" s="6"/>
+      <c r="BV11">
+        <v>34</v>
+      </c>
+      <c r="BW11">
+        <v>7</v>
+      </c>
+      <c r="BY11">
+        <f t="shared" si="5"/>
+        <v>136</v>
+      </c>
+      <c r="BZ11">
+        <f t="shared" si="6"/>
+        <v>52</v>
+      </c>
+      <c r="CC11" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([136,52])</v>
+      </c>
+    </row>
+    <row r="12" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4"/>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AU12">
+        <v>15</v>
+      </c>
+      <c r="AV12">
+        <v>8</v>
+      </c>
+      <c r="AW12">
+        <v>16</v>
+      </c>
+      <c r="AX12">
+        <v>15</v>
+      </c>
+      <c r="AZ12">
+        <f t="shared" si="9"/>
+        <v>60</v>
+      </c>
+      <c r="BA12">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="BB12">
+        <f t="shared" si="8"/>
+        <v>64</v>
+      </c>
+      <c r="BC12">
+        <f t="shared" si="11"/>
+        <v>48</v>
+      </c>
+      <c r="BE12" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(60,20),Vector2d(64,48))</v>
+      </c>
+      <c r="BF12" s="6"/>
+      <c r="BV12">
+        <v>16</v>
+      </c>
+      <c r="BW12">
+        <v>8</v>
+      </c>
+      <c r="BY12">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="BZ12">
+        <f t="shared" si="6"/>
+        <v>48</v>
+      </c>
+      <c r="CC12" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([64,48])</v>
+      </c>
+    </row>
+    <row r="13" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+      <c r="AU13">
+        <v>19</v>
+      </c>
+      <c r="AV13">
+        <v>6</v>
+      </c>
+      <c r="AW13">
+        <v>20</v>
+      </c>
+      <c r="AX13">
+        <v>13</v>
+      </c>
+      <c r="AZ13">
+        <f t="shared" si="9"/>
+        <v>76</v>
+      </c>
+      <c r="BA13">
+        <f t="shared" si="10"/>
+        <v>28</v>
+      </c>
+      <c r="BB13">
+        <f t="shared" si="8"/>
+        <v>80</v>
+      </c>
+      <c r="BC13">
+        <f t="shared" si="11"/>
+        <v>56</v>
+      </c>
+      <c r="BE13" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(76,28),Vector2d(80,56))</v>
+      </c>
+      <c r="BF13" s="6"/>
+      <c r="BV13">
+        <v>20</v>
+      </c>
+      <c r="BW13">
+        <v>8</v>
+      </c>
+      <c r="BY13">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="BZ13">
+        <f t="shared" si="6"/>
+        <v>48</v>
+      </c>
+      <c r="CC13" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([80,48])</v>
+      </c>
+    </row>
+    <row r="14" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AU14">
+        <v>15</v>
+      </c>
+      <c r="AV14">
+        <v>12</v>
+      </c>
+      <c r="AW14">
+        <v>22</v>
+      </c>
+      <c r="AX14">
+        <v>13</v>
+      </c>
+      <c r="AZ14">
+        <f t="shared" si="9"/>
+        <v>60</v>
+      </c>
+      <c r="BA14">
+        <f t="shared" si="10"/>
+        <v>28</v>
+      </c>
+      <c r="BB14">
+        <f t="shared" si="8"/>
+        <v>88</v>
+      </c>
+      <c r="BC14">
+        <f t="shared" si="11"/>
+        <v>32</v>
+      </c>
+      <c r="BE14" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(60,28),Vector2d(88,32))</v>
+      </c>
+      <c r="BF14" s="6"/>
+      <c r="BV14">
+        <v>29</v>
+      </c>
+      <c r="BW14">
+        <v>9</v>
+      </c>
+      <c r="BY14">
+        <f t="shared" si="5"/>
+        <v>116</v>
+      </c>
+      <c r="BZ14">
+        <f t="shared" si="6"/>
+        <v>44</v>
+      </c>
+      <c r="CC14" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([116,44])</v>
+      </c>
+    </row>
+    <row r="15" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
+      <c r="AU15">
+        <v>23</v>
+      </c>
+      <c r="AV15">
+        <v>12</v>
+      </c>
+      <c r="AW15">
+        <v>36</v>
+      </c>
+      <c r="AX15">
+        <v>13</v>
+      </c>
+      <c r="AZ15">
+        <f t="shared" si="9"/>
+        <v>92</v>
+      </c>
+      <c r="BA15">
+        <f t="shared" si="10"/>
+        <v>28</v>
+      </c>
+      <c r="BB15">
+        <f t="shared" si="8"/>
+        <v>144</v>
+      </c>
+      <c r="BC15">
+        <f t="shared" si="11"/>
+        <v>32</v>
+      </c>
+      <c r="BE15" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(92,28),Vector2d(144,32))</v>
+      </c>
+      <c r="BF15" s="6"/>
+      <c r="BV15">
+        <v>32</v>
+      </c>
+      <c r="BW15">
+        <v>9</v>
+      </c>
+      <c r="BY15">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+      <c r="BZ15">
+        <f t="shared" si="6"/>
+        <v>44</v>
+      </c>
+      <c r="CC15" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([128,44])</v>
+      </c>
+    </row>
+    <row r="16" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AU16">
+        <v>19</v>
+      </c>
+      <c r="AV16">
+        <v>7</v>
+      </c>
+      <c r="AW16">
+        <v>23</v>
+      </c>
+      <c r="AX16">
+        <v>8</v>
+      </c>
+      <c r="AZ16">
+        <f t="shared" si="9"/>
+        <v>76</v>
+      </c>
+      <c r="BA16">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="BB16">
+        <f t="shared" si="8"/>
+        <v>92</v>
+      </c>
+      <c r="BC16">
+        <f t="shared" si="11"/>
+        <v>52</v>
+      </c>
+      <c r="BE16" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(76,48),Vector2d(92,52))</v>
+      </c>
+      <c r="BF16" s="6"/>
+      <c r="BV16">
+        <v>25</v>
+      </c>
+      <c r="BW16">
+        <v>10</v>
+      </c>
+      <c r="BY16">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="BZ16">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="CC16" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([100,40])</v>
+      </c>
+    </row>
+    <row r="17" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+      <c r="AU17">
+        <v>24</v>
+      </c>
+      <c r="AV17">
+        <v>7</v>
+      </c>
+      <c r="AW17">
+        <v>32</v>
+      </c>
+      <c r="AX17">
+        <v>8</v>
+      </c>
+      <c r="AZ17">
+        <f t="shared" si="9"/>
+        <v>96</v>
+      </c>
+      <c r="BA17">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="BB17">
+        <f t="shared" si="8"/>
+        <v>128</v>
+      </c>
+      <c r="BC17">
+        <f t="shared" si="11"/>
+        <v>52</v>
+      </c>
+      <c r="BE17" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(96,48),Vector2d(128,52))</v>
+      </c>
+      <c r="BF17" s="6"/>
+      <c r="BV17">
+        <v>5</v>
+      </c>
+      <c r="BW17">
+        <v>11</v>
+      </c>
+      <c r="BY17">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="BZ17">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+      <c r="CC17" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([20,36])</v>
+      </c>
+    </row>
+    <row r="18" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+      <c r="AU18">
+        <v>8</v>
+      </c>
+      <c r="AV18">
+        <v>12</v>
+      </c>
+      <c r="AW18">
+        <v>9</v>
+      </c>
+      <c r="AX18">
+        <v>13</v>
+      </c>
+      <c r="AZ18">
+        <f t="shared" si="9"/>
+        <v>32</v>
+      </c>
+      <c r="BA18">
+        <f t="shared" si="10"/>
+        <v>28</v>
+      </c>
+      <c r="BB18">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="BC18">
+        <f t="shared" si="11"/>
+        <v>32</v>
+      </c>
+      <c r="BE18" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(32,28),Vector2d(36,32))</v>
+      </c>
+      <c r="BV18">
+        <v>9</v>
+      </c>
+      <c r="BW18">
+        <v>11</v>
+      </c>
+      <c r="BY18">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="BZ18">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+      <c r="CC18" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([36,36])</v>
+      </c>
+    </row>
+    <row r="19" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="AU19">
+        <v>12</v>
+      </c>
+      <c r="AV19">
+        <v>12</v>
+      </c>
+      <c r="AW19">
+        <v>13</v>
+      </c>
+      <c r="AX19">
+        <v>13</v>
+      </c>
+      <c r="AZ19">
+        <f t="shared" si="9"/>
+        <v>48</v>
+      </c>
+      <c r="BA19">
+        <f t="shared" si="10"/>
+        <v>28</v>
+      </c>
+      <c r="BB19">
+        <f t="shared" si="8"/>
+        <v>52</v>
+      </c>
+      <c r="BC19">
+        <f t="shared" si="11"/>
+        <v>32</v>
+      </c>
+      <c r="BE19" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(48,28),Vector2d(52,32))</v>
+      </c>
+      <c r="BV19">
+        <v>13</v>
+      </c>
+      <c r="BW19">
+        <v>11</v>
+      </c>
+      <c r="BY19">
+        <f t="shared" si="5"/>
+        <v>52</v>
+      </c>
+      <c r="BZ19">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+      <c r="CC19" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([52,36])</v>
+      </c>
+    </row>
+    <row r="20" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="AU20">
+        <v>8</v>
+      </c>
+      <c r="AV20">
+        <v>15</v>
+      </c>
+      <c r="AW20">
+        <v>11</v>
+      </c>
+      <c r="AX20">
+        <v>16</v>
+      </c>
+      <c r="AZ20">
+        <f t="shared" si="9"/>
+        <v>32</v>
+      </c>
+      <c r="BA20">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="BB20">
+        <f t="shared" si="8"/>
+        <v>44</v>
+      </c>
+      <c r="BC20">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="BE20" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(32,16),Vector2d(44,20))</v>
+      </c>
+      <c r="BV20">
+        <v>18</v>
+      </c>
+      <c r="BW20">
+        <v>11</v>
+      </c>
+      <c r="BY20">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="BZ20">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+      <c r="CC20" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([72,36])</v>
+      </c>
+    </row>
+    <row r="21" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AU21">
+        <v>12</v>
+      </c>
+      <c r="AV21">
+        <v>15</v>
+      </c>
+      <c r="AW21">
+        <v>15</v>
+      </c>
+      <c r="AX21">
+        <v>16</v>
+      </c>
+      <c r="AZ21">
+        <f t="shared" si="9"/>
+        <v>48</v>
+      </c>
+      <c r="BA21">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="BB21">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="BC21">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="BE21" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(48,16),Vector2d(60,20))</v>
+      </c>
+      <c r="BV21">
+        <v>17</v>
+      </c>
+      <c r="BW21">
+        <v>14</v>
+      </c>
+      <c r="BY21">
+        <f t="shared" si="5"/>
+        <v>68</v>
+      </c>
+      <c r="BZ21">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="CC21" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([68,24])</v>
+      </c>
+    </row>
+    <row r="22" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AU22">
+        <v>8</v>
+      </c>
+      <c r="AV22">
+        <v>7</v>
+      </c>
+      <c r="AW22">
+        <v>11</v>
+      </c>
+      <c r="AX22">
+        <v>8</v>
+      </c>
+      <c r="AZ22">
+        <f t="shared" si="9"/>
+        <v>32</v>
+      </c>
+      <c r="BA22">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="BB22">
+        <f t="shared" si="8"/>
+        <v>44</v>
+      </c>
+      <c r="BC22">
+        <f t="shared" si="11"/>
+        <v>52</v>
+      </c>
+      <c r="BE22" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(32,48),Vector2d(44,52))</v>
+      </c>
+      <c r="BV22">
+        <v>21</v>
+      </c>
+      <c r="BW22">
+        <v>14</v>
+      </c>
+      <c r="BY22">
+        <f t="shared" si="5"/>
+        <v>84</v>
+      </c>
+      <c r="BZ22">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="CC22" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([84,24])</v>
+      </c>
+    </row>
+    <row r="23" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AU23">
+        <v>12</v>
+      </c>
+      <c r="AV23">
+        <v>7</v>
+      </c>
+      <c r="AW23">
+        <v>15</v>
+      </c>
+      <c r="AX23">
+        <v>8</v>
+      </c>
+      <c r="AZ23">
+        <f t="shared" si="9"/>
+        <v>48</v>
+      </c>
+      <c r="BA23">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="BB23">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="BC23">
+        <f t="shared" si="11"/>
+        <v>52</v>
+      </c>
+      <c r="BE23" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(48,48),Vector2d(60,52))</v>
+      </c>
+      <c r="BV23">
+        <v>25</v>
+      </c>
+      <c r="BW23">
+        <v>14</v>
+      </c>
+      <c r="BY23">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="BZ23">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="CC23" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([100,24])</v>
+      </c>
+    </row>
+    <row r="24" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AU24">
+        <v>9</v>
+      </c>
+      <c r="AV24">
+        <v>9</v>
+      </c>
+      <c r="AW24">
+        <v>10</v>
+      </c>
+      <c r="AX24">
+        <v>11</v>
+      </c>
+      <c r="AZ24">
+        <f t="shared" si="9"/>
+        <v>36</v>
+      </c>
+      <c r="BA24">
+        <f t="shared" si="10"/>
+        <v>36</v>
+      </c>
+      <c r="BB24">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="BC24">
+        <f t="shared" si="11"/>
+        <v>44</v>
+      </c>
+      <c r="BE24" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(36,36),Vector2d(40,44))</v>
+      </c>
+      <c r="BV24">
+        <v>29</v>
+      </c>
+      <c r="BW24">
+        <v>14</v>
+      </c>
+      <c r="BY24">
+        <f t="shared" si="5"/>
+        <v>116</v>
+      </c>
+      <c r="BZ24">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="CC24" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([116,24])</v>
+      </c>
+    </row>
+    <row r="25" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AU25">
+        <v>13</v>
+      </c>
+      <c r="AV25">
+        <v>9</v>
+      </c>
+      <c r="AW25">
+        <v>14</v>
+      </c>
+      <c r="AX25">
+        <v>11</v>
+      </c>
+      <c r="AZ25">
+        <f t="shared" si="9"/>
+        <v>52</v>
+      </c>
+      <c r="BA25">
+        <f t="shared" si="10"/>
+        <v>36</v>
+      </c>
+      <c r="BB25">
+        <f t="shared" si="8"/>
+        <v>56</v>
+      </c>
+      <c r="BC25">
+        <f t="shared" si="11"/>
+        <v>44</v>
+      </c>
+      <c r="BE25" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(52,36),Vector2d(56,44))</v>
+      </c>
+      <c r="BV25">
+        <v>33</v>
+      </c>
+      <c r="BW25">
+        <v>14</v>
+      </c>
+      <c r="BY25">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+      <c r="BZ25">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="CC25" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([132,24])</v>
+      </c>
+    </row>
+    <row r="26" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AU26">
+        <v>17</v>
+      </c>
+      <c r="AV26">
+        <v>9</v>
+      </c>
+      <c r="AW26">
+        <v>18</v>
+      </c>
+      <c r="AX26">
+        <v>11</v>
+      </c>
+      <c r="AZ26">
+        <f t="shared" si="9"/>
+        <v>68</v>
+      </c>
+      <c r="BA26">
+        <f t="shared" si="10"/>
+        <v>36</v>
+      </c>
+      <c r="BB26">
+        <f t="shared" si="8"/>
+        <v>72</v>
+      </c>
+      <c r="BC26">
+        <f t="shared" si="11"/>
+        <v>44</v>
+      </c>
+      <c r="BE26" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(68,36),Vector2d(72,44))</v>
+      </c>
+      <c r="BV26">
+        <v>5</v>
+      </c>
+      <c r="BW26">
+        <v>17</v>
+      </c>
+      <c r="BY26">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="BZ26">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="CC26" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([20,12])</v>
+      </c>
+    </row>
+    <row r="27" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AU27">
+        <v>23</v>
+      </c>
+      <c r="AV27">
+        <v>8</v>
+      </c>
+      <c r="AW27">
+        <v>24</v>
+      </c>
+      <c r="AX27">
+        <v>12</v>
+      </c>
+      <c r="AZ27">
+        <f t="shared" si="9"/>
+        <v>92</v>
+      </c>
+      <c r="BA27">
+        <f t="shared" si="10"/>
+        <v>32</v>
+      </c>
+      <c r="BB27">
+        <f t="shared" si="8"/>
+        <v>96</v>
+      </c>
+      <c r="BC27">
+        <f t="shared" si="11"/>
+        <v>48</v>
+      </c>
+      <c r="BE27" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(92,32),Vector2d(96,48))</v>
+      </c>
+      <c r="BV27">
+        <v>9</v>
+      </c>
+      <c r="BW27">
+        <v>17</v>
+      </c>
+      <c r="BY27">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="BZ27">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="CC27" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([36,12])</v>
+      </c>
+    </row>
+    <row r="28" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AU28">
+        <v>27</v>
+      </c>
+      <c r="AV28">
+        <v>8</v>
+      </c>
+      <c r="AW28">
+        <v>28</v>
+      </c>
+      <c r="AX28">
+        <v>12</v>
+      </c>
+      <c r="AZ28">
+        <f t="shared" si="9"/>
+        <v>108</v>
+      </c>
+      <c r="BA28">
+        <f t="shared" si="10"/>
+        <v>32</v>
+      </c>
+      <c r="BB28">
+        <f t="shared" si="8"/>
+        <v>112</v>
+      </c>
+      <c r="BC28">
+        <f t="shared" si="11"/>
+        <v>48</v>
+      </c>
+      <c r="BE28" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(108,32),Vector2d(112,48))</v>
+      </c>
+      <c r="BV28">
+        <v>13</v>
+      </c>
+      <c r="BW28">
+        <v>17</v>
+      </c>
+      <c r="BY28">
+        <f t="shared" si="5"/>
+        <v>52</v>
+      </c>
+      <c r="BZ28">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="CC28" t="str">
+        <f t="shared" si="7"/>
+        <v>locations.append([52,12])</v>
+      </c>
+    </row>
+    <row r="29" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AU29">
+        <v>31</v>
+      </c>
+      <c r="AV29">
+        <v>6</v>
+      </c>
+      <c r="AW29">
+        <v>32</v>
+      </c>
+      <c r="AX29">
+        <v>12</v>
+      </c>
+      <c r="AZ29">
+        <f t="shared" si="9"/>
+        <v>124</v>
+      </c>
+      <c r="BA29">
+        <f t="shared" si="10"/>
+        <v>32</v>
+      </c>
+      <c r="BB29">
+        <f t="shared" si="8"/>
+        <v>128</v>
+      </c>
+      <c r="BC29">
+        <f t="shared" si="11"/>
+        <v>56</v>
+      </c>
+      <c r="BE29" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(124,32),Vector2d(128,56))</v>
+      </c>
+      <c r="BY29">
+        <f t="shared" ref="BY29:BY35" si="13">BV29*4</f>
+        <v>0</v>
+      </c>
+      <c r="BZ29">
+        <f t="shared" ref="BZ29:BZ35" si="14">4*(20-BW29)</f>
+        <v>80</v>
+      </c>
+      <c r="CC29" t="str">
+        <f t="shared" ref="CC29:CC35" si="15">"locations.append(["&amp;BY29&amp;","&amp;BZ29&amp;"])"</f>
+        <v>locations.append([0,80])</v>
+      </c>
+    </row>
+    <row r="30" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AU30">
+        <v>33</v>
+      </c>
+      <c r="AV30">
+        <v>6</v>
+      </c>
+      <c r="AW30">
+        <v>34</v>
+      </c>
+      <c r="AX30">
+        <v>12</v>
+      </c>
+      <c r="AZ30">
+        <f t="shared" si="9"/>
+        <v>132</v>
+      </c>
+      <c r="BA30">
+        <f t="shared" si="10"/>
+        <v>32</v>
+      </c>
+      <c r="BB30">
+        <f t="shared" si="8"/>
+        <v>136</v>
+      </c>
+      <c r="BC30">
+        <f t="shared" si="11"/>
+        <v>56</v>
+      </c>
+      <c r="BE30" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(132,32),Vector2d(136,56))</v>
+      </c>
+      <c r="BV30">
+        <v>2</v>
+      </c>
+      <c r="BW30">
+        <v>4</v>
+      </c>
+      <c r="BY30">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="BZ30">
+        <f t="shared" si="14"/>
+        <v>64</v>
+      </c>
+      <c r="CC30" t="str">
+        <f t="shared" si="15"/>
+        <v>locations.append([8,64])</v>
+      </c>
+    </row>
+    <row r="31" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AU31">
+        <v>35</v>
+      </c>
+      <c r="AV31">
+        <v>6</v>
+      </c>
+      <c r="AW31">
+        <v>36</v>
+      </c>
+      <c r="AX31">
+        <v>12</v>
+      </c>
+      <c r="AZ31">
+        <f t="shared" si="9"/>
+        <v>140</v>
+      </c>
+      <c r="BA31">
+        <f t="shared" si="10"/>
+        <v>32</v>
+      </c>
+      <c r="BB31">
+        <f t="shared" si="8"/>
+        <v>144</v>
+      </c>
+      <c r="BC31">
+        <f t="shared" si="11"/>
+        <v>56</v>
+      </c>
+      <c r="BE31" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(140,32),Vector2d(144,56))</v>
+      </c>
+      <c r="BV31">
+        <v>2</v>
+      </c>
+      <c r="BW31">
+        <v>12</v>
+      </c>
+      <c r="BY31">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="BZ31">
+        <f t="shared" si="14"/>
+        <v>32</v>
+      </c>
+      <c r="CC31" t="str">
+        <f t="shared" si="15"/>
+        <v>locations.append([8,32])</v>
+      </c>
+    </row>
+    <row r="32" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="AU32">
+        <v>21</v>
+      </c>
+      <c r="AV32">
+        <v>11</v>
+      </c>
+      <c r="AW32">
+        <v>22</v>
+      </c>
+      <c r="AX32">
+        <v>12</v>
+      </c>
+      <c r="AZ32">
+        <f t="shared" si="9"/>
+        <v>84</v>
+      </c>
+      <c r="BA32">
+        <f t="shared" si="10"/>
+        <v>32</v>
+      </c>
+      <c r="BB32">
+        <f t="shared" si="8"/>
+        <v>88</v>
+      </c>
+      <c r="BC32">
+        <f t="shared" si="11"/>
+        <v>36</v>
+      </c>
+      <c r="BE32" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(84,32),Vector2d(88,36))</v>
+      </c>
+      <c r="BV32">
+        <v>2</v>
+      </c>
+      <c r="BW32">
+        <v>17</v>
+      </c>
+      <c r="BY32">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="BZ32">
+        <f t="shared" si="14"/>
+        <v>12</v>
+      </c>
+      <c r="CC32" t="str">
+        <f t="shared" si="15"/>
+        <v>locations.append([8,12])</v>
+      </c>
+    </row>
+    <row r="33" spans="47:81" x14ac:dyDescent="0.25">
+      <c r="AU33">
+        <v>22</v>
+      </c>
+      <c r="AV33">
+        <v>10</v>
+      </c>
+      <c r="AW33">
+        <v>23</v>
+      </c>
+      <c r="AX33">
+        <v>11</v>
+      </c>
+      <c r="AZ33">
+        <f t="shared" si="9"/>
+        <v>88</v>
+      </c>
+      <c r="BA33">
+        <f t="shared" si="10"/>
+        <v>36</v>
+      </c>
+      <c r="BB33">
+        <f t="shared" si="8"/>
+        <v>92</v>
+      </c>
+      <c r="BC33">
+        <f t="shared" si="11"/>
+        <v>40</v>
+      </c>
+      <c r="BE33" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(88,36),Vector2d(92,40))</v>
+      </c>
+      <c r="BV33">
+        <v>10</v>
+      </c>
+      <c r="BW33">
+        <v>8</v>
+      </c>
+      <c r="BY33">
+        <f t="shared" si="13"/>
+        <v>40</v>
+      </c>
+      <c r="BZ33">
+        <f t="shared" si="14"/>
+        <v>48</v>
+      </c>
+      <c r="CC33" t="str">
+        <f t="shared" si="15"/>
+        <v>locations.append([40,48])</v>
+      </c>
+    </row>
+    <row r="34" spans="47:81" x14ac:dyDescent="0.25">
+      <c r="AU34">
+        <v>25</v>
+      </c>
+      <c r="AV34">
+        <v>9</v>
+      </c>
+      <c r="AW34">
+        <v>26</v>
+      </c>
+      <c r="AX34">
+        <v>10</v>
+      </c>
+      <c r="AZ34">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="BA34">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="BB34">
+        <f t="shared" si="8"/>
+        <v>104</v>
+      </c>
+      <c r="BC34">
+        <f t="shared" si="11"/>
+        <v>44</v>
+      </c>
+      <c r="BE34" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(100,40),Vector2d(104,44))</v>
+      </c>
+      <c r="BV34">
+        <v>14</v>
+      </c>
+      <c r="BW34">
+        <v>8</v>
+      </c>
+      <c r="BY34">
+        <f t="shared" si="13"/>
+        <v>56</v>
+      </c>
+      <c r="BZ34">
+        <f t="shared" si="14"/>
+        <v>48</v>
+      </c>
+      <c r="CC34" t="str">
+        <f t="shared" si="15"/>
+        <v>locations.append([56,48])</v>
+      </c>
+    </row>
+    <row r="35" spans="47:81" x14ac:dyDescent="0.25">
+      <c r="AU35">
+        <v>28</v>
+      </c>
+      <c r="AV35">
+        <v>10</v>
+      </c>
+      <c r="AW35">
+        <v>29</v>
+      </c>
+      <c r="AX35">
+        <v>11</v>
+      </c>
+      <c r="AZ35">
+        <f t="shared" si="9"/>
+        <v>112</v>
+      </c>
+      <c r="BA35">
+        <f t="shared" si="10"/>
+        <v>36</v>
+      </c>
+      <c r="BB35">
+        <f t="shared" si="8"/>
+        <v>116</v>
+      </c>
+      <c r="BC35">
+        <f t="shared" si="11"/>
+        <v>40</v>
+      </c>
+      <c r="BE35" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(112,36),Vector2d(116,40))</v>
+      </c>
+      <c r="BV35">
+        <v>30</v>
+      </c>
+      <c r="BW35">
+        <v>11</v>
+      </c>
+      <c r="BY35">
+        <f t="shared" si="13"/>
+        <v>120</v>
+      </c>
+      <c r="BZ35">
+        <f t="shared" si="14"/>
+        <v>36</v>
+      </c>
+      <c r="CC35" t="str">
+        <f t="shared" si="15"/>
+        <v>locations.append([120,36])</v>
+      </c>
+    </row>
+    <row r="36" spans="47:81" x14ac:dyDescent="0.25">
+      <c r="AU36">
+        <v>30</v>
+      </c>
+      <c r="AV36">
+        <v>9</v>
+      </c>
+      <c r="AW36">
+        <v>31</v>
+      </c>
+      <c r="AX36">
+        <v>10</v>
+      </c>
+      <c r="AZ36">
+        <f t="shared" si="9"/>
+        <v>120</v>
+      </c>
+      <c r="BA36">
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="BB36">
+        <f t="shared" si="8"/>
+        <v>124</v>
+      </c>
+      <c r="BC36">
+        <f t="shared" si="11"/>
+        <v>44</v>
+      </c>
+      <c r="BE36" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(120,40),Vector2d(124,44))</v>
+      </c>
+    </row>
+    <row r="37" spans="47:81" x14ac:dyDescent="0.25">
+      <c r="AU37">
+        <v>32</v>
+      </c>
+      <c r="AV37">
+        <v>8</v>
+      </c>
+      <c r="AW37">
+        <v>33</v>
+      </c>
+      <c r="AX37">
+        <v>9</v>
+      </c>
+      <c r="AZ37">
+        <f t="shared" si="9"/>
+        <v>128</v>
+      </c>
+      <c r="BA37">
+        <f t="shared" si="10"/>
+        <v>44</v>
+      </c>
+      <c r="BB37">
+        <f t="shared" si="8"/>
+        <v>132</v>
+      </c>
+      <c r="BC37">
+        <f t="shared" si="11"/>
+        <v>48</v>
+      </c>
+      <c r="BE37" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(128,44),Vector2d(132,48))</v>
+      </c>
+    </row>
+    <row r="38" spans="47:81" x14ac:dyDescent="0.25">
+      <c r="AU38">
+        <v>32</v>
+      </c>
+      <c r="AV38">
+        <v>5</v>
+      </c>
+      <c r="AW38">
+        <v>33</v>
+      </c>
+      <c r="AX38">
+        <v>6</v>
+      </c>
+      <c r="AZ38">
+        <f t="shared" si="9"/>
+        <v>128</v>
+      </c>
+      <c r="BA38">
+        <f t="shared" si="10"/>
+        <v>56</v>
+      </c>
+      <c r="BB38">
+        <f t="shared" si="8"/>
+        <v>132</v>
+      </c>
+      <c r="BC38">
+        <f t="shared" si="11"/>
+        <v>60</v>
+      </c>
+      <c r="BE38" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(128,56),Vector2d(132,60))</v>
+      </c>
+    </row>
+    <row r="39" spans="47:81" x14ac:dyDescent="0.25">
+      <c r="AU39">
+        <v>34</v>
+      </c>
+      <c r="AV39">
+        <v>5</v>
+      </c>
+      <c r="AW39">
+        <v>35</v>
+      </c>
+      <c r="AX39">
+        <v>6</v>
+      </c>
+      <c r="AZ39">
+        <f t="shared" si="9"/>
+        <v>136</v>
+      </c>
+      <c r="BA39">
+        <f t="shared" si="10"/>
+        <v>56</v>
+      </c>
+      <c r="BB39">
+        <f t="shared" si="8"/>
+        <v>140</v>
+      </c>
+      <c r="BC39">
+        <f t="shared" si="11"/>
+        <v>60</v>
+      </c>
+      <c r="BE39" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(136,56),Vector2d(140,60))</v>
+      </c>
+    </row>
+    <row r="40" spans="47:81" x14ac:dyDescent="0.25">
+      <c r="AU40">
+        <v>18</v>
+      </c>
+      <c r="AV40">
+        <v>5</v>
+      </c>
+      <c r="AW40">
+        <v>19</v>
+      </c>
+      <c r="AX40">
+        <v>6</v>
+      </c>
+      <c r="AZ40">
+        <f t="shared" si="9"/>
+        <v>72</v>
+      </c>
+      <c r="BA40">
+        <f t="shared" si="10"/>
+        <v>56</v>
+      </c>
+      <c r="BB40">
+        <f t="shared" si="8"/>
+        <v>76</v>
+      </c>
+      <c r="BC40">
+        <f t="shared" si="11"/>
+        <v>60</v>
+      </c>
+      <c r="BE40" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(72,56),Vector2d(76,60))</v>
+      </c>
+    </row>
+    <row r="41" spans="47:81" x14ac:dyDescent="0.25">
+      <c r="AU41">
+        <v>17</v>
+      </c>
+      <c r="AV41">
+        <v>6</v>
+      </c>
+      <c r="AW41">
+        <v>18</v>
+      </c>
+      <c r="AX41">
+        <v>8</v>
+      </c>
+      <c r="AZ41">
+        <f t="shared" si="9"/>
+        <v>68</v>
+      </c>
+      <c r="BA41">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="BB41">
+        <f t="shared" si="8"/>
+        <v>72</v>
+      </c>
+      <c r="BC41">
+        <f t="shared" si="11"/>
+        <v>56</v>
+      </c>
+      <c r="BE41" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(68,48),Vector2d(72,56))</v>
+      </c>
+    </row>
+    <row r="42" spans="47:81" x14ac:dyDescent="0.25">
+      <c r="AU42">
+        <v>16</v>
+      </c>
+      <c r="AV42">
+        <v>7</v>
+      </c>
+      <c r="AW42">
+        <v>18</v>
+      </c>
+      <c r="AX42">
+        <v>8</v>
+      </c>
+      <c r="AZ42">
+        <f t="shared" si="9"/>
+        <v>64</v>
+      </c>
+      <c r="BA42">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="BB42">
+        <f t="shared" si="8"/>
+        <v>72</v>
+      </c>
+      <c r="BC42">
+        <f t="shared" si="11"/>
+        <v>52</v>
+      </c>
+      <c r="BE42" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>box.addBox(Vector2d(64,48),Vector2d(72,52))</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="BV1:BW31">
+    <sortCondition ref="BW1:BW31"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>